<commit_message>
code list v3.x fixed
</commit_message>
<xml_diff>
--- a/ESPD/codelists/ESPD-CodeLists_v3.1.0.xlsx
+++ b/ESPD/codelists/ESPD-CodeLists_v3.1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STOICDR\Documents\espd-demo\ESPD\codelists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F1BF96-0AA6-4CE5-9A24-9A0B6EA41C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2230203-CA8E-4E66-AE6E-46BF4579B0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -919,9 +919,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM</t>
-  </si>
-  <si>
     <t>BACH Banque de France</t>
   </si>
   <si>
@@ -1306,33 +1303,9 @@
     <t>3.1.0</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/CriterionElementType.gc</t>
-  </si>
-  <si>
     <t>https://github.com/OP-TED/ESPD-EDM/tree/3.1.0/</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/BooleanGUIControlType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/EOIDType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/FinancialRatioType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ProfileExecutionID.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/PropertyGroupType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ResponseDataType.gc</t>
-  </si>
-  <si>
     <t>ESPD-EDMv3.1.0</t>
   </si>
   <si>
@@ -1340,6 +1313,33 @@
   </si>
   <si>
     <t>http://publications.europa.eu/resource/distribution/access-right/20220316-0/xml/gc/AccessRight.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0/codelists/gc/BooleanGUIControlType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0/codelists/gc/CriterionElementType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0/codelists/gc/EOIDType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0/codelists/gc/FinancialRatioType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0/codelists/gc/ProfileExecutionID.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0/codelists/gc/PropertyGroupType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/v3.1.0/codelists/gc/ResponseDataType.gc</t>
   </si>
 </sst>
 </file>
@@ -7056,7 +7056,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -7067,7 +7067,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -7076,7 +7076,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -7085,7 +7085,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -7094,7 +7094,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -7103,7 +7103,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -7112,7 +7112,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
@@ -7122,7 +7122,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -7131,7 +7131,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -7140,7 +7140,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -7232,42 +7232,42 @@
     </row>
     <row r="11" spans="1:28">
       <c r="A11" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>300</v>
-      </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:28">
       <c r="A12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B12" t="s">
         <v>301</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>303</v>
-      </c>
       <c r="D12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -7322,7 +7322,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7330,7 +7330,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7338,7 +7338,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7346,7 +7346,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7354,7 +7354,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7362,7 +7362,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -7370,7 +7370,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -7378,7 +7378,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -7386,7 +7386,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -7428,7 +7428,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -7436,7 +7436,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -7444,7 +7444,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -7452,7 +7452,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -7460,7 +7460,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -7468,7 +7468,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -7576,7 +7576,7 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I10" s="6"/>
       <c r="L10" t="s">
@@ -7594,7 +7594,7 @@
         <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L11" t="s">
         <v>58</v>
@@ -7611,7 +7611,7 @@
         <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L12" t="s">
         <v>60</v>
@@ -7628,7 +7628,7 @@
         <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L13" t="s">
         <v>62</v>
@@ -7645,7 +7645,7 @@
         <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L14" t="s">
         <v>64</v>
@@ -7662,7 +7662,7 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L15" t="s">
         <v>66</v>
@@ -7679,7 +7679,7 @@
         <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L16" t="s">
         <v>75</v>
@@ -7696,7 +7696,7 @@
         <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L17" t="s">
         <v>76</v>
@@ -7713,7 +7713,7 @@
         <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L18" t="s">
         <v>78</v>
@@ -7730,7 +7730,7 @@
         <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L19" t="s">
         <v>80</v>
@@ -7747,7 +7747,7 @@
         <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L20" t="s">
         <v>82</v>
@@ -7764,7 +7764,7 @@
         <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L21" t="s">
         <v>84</v>
@@ -7781,7 +7781,7 @@
         <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L22" t="s">
         <v>86</v>
@@ -7798,7 +7798,7 @@
         <v>97</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -7822,7 +7822,7 @@
         <v>99</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -7862,7 +7862,7 @@
         <v>101</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -7902,7 +7902,7 @@
         <v>102</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -7942,7 +7942,7 @@
         <v>103</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -7982,7 +7982,7 @@
         <v>104</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -8022,7 +8022,7 @@
         <v>105</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -8062,7 +8062,7 @@
         <v>107</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -8102,7 +8102,7 @@
         <v>109</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -8142,7 +8142,7 @@
         <v>111</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -8182,7 +8182,7 @@
         <v>115</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -8222,7 +8222,7 @@
         <v>117</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -8262,7 +8262,7 @@
         <v>122</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -8302,7 +8302,7 @@
         <v>123</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -8342,7 +8342,7 @@
         <v>124</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -8382,7 +8382,7 @@
         <v>125</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -8413,9 +8413,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId1" display="https://github.com/ESPD/ESPD-EDM" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/FinancialRatioType.gc" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -8446,7 +8446,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -8455,7 +8455,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -8464,7 +8464,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -8472,7 +8472,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8481,7 +8481,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -8490,7 +8490,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8499,7 +8499,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8508,7 +8508,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -8517,7 +8517,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -8554,7 +8554,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -8563,7 +8563,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -8572,7 +8572,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -8581,7 +8581,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8590,7 +8590,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -8599,7 +8599,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8608,7 +8608,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8617,7 +8617,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -8651,7 +8651,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -8686,7 +8686,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -8696,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -8706,7 +8706,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -8716,7 +8716,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -8726,7 +8726,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -8736,7 +8736,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -8829,139 +8829,139 @@
     </row>
     <row r="8" spans="1:28">
       <c r="A8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
         <v>206</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>207</v>
       </c>
-      <c r="C8" t="s">
-        <v>208</v>
-      </c>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G8" s="6"/>
       <c r="L8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:28">
       <c r="A9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" t="s">
         <v>209</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>210</v>
       </c>
-      <c r="C9" t="s">
-        <v>211</v>
-      </c>
       <c r="D9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="14.25">
       <c r="A10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="14.25">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J11" s="6"/>
       <c r="L11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="14.25">
       <c r="A12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" t="s">
         <v>212</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>213</v>
       </c>
-      <c r="C12" t="s">
-        <v>214</v>
-      </c>
       <c r="D12" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="14.25">
       <c r="A13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" t="s">
         <v>246</v>
       </c>
-      <c r="B13" t="s">
-        <v>247</v>
-      </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F13" s="6"/>
       <c r="J13" s="6"/>
       <c r="L13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="14.25">
       <c r="A14" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="14.25">
       <c r="A15" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>251</v>
-      </c>
       <c r="D15" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -8971,7 +8971,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
@@ -8992,16 +8992,16 @@
     </row>
     <row r="16" spans="1:28" ht="14.25">
       <c r="A16" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>307</v>
-      </c>
       <c r="D16" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -9011,7 +9011,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -9032,25 +9032,25 @@
     </row>
     <row r="17" spans="1:12" ht="14.25">
       <c r="A17" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B17" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C17" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L17" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ProfileExecutionID.gc" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -9085,7 +9085,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -9094,7 +9094,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -9103,7 +9103,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="C4" s="14"/>
     </row>
@@ -9112,7 +9112,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -9121,7 +9121,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -9222,7 +9222,7 @@
         <v>162</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -9262,7 +9262,7 @@
         <v>163</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -9302,7 +9302,7 @@
         <v>164</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -9333,8 +9333,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/PropertyGroupType.gc" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -9373,7 +9373,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -9383,7 +9383,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -9393,7 +9393,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -9403,7 +9403,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -9413,7 +9413,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -9515,7 +9515,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -9555,7 +9555,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="10"/>
@@ -9595,7 +9595,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -9629,13 +9629,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -9645,7 +9645,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -9675,7 +9675,7 @@
         <v>20</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -9715,7 +9715,7 @@
         <v>167</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -9755,7 +9755,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -9795,7 +9795,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -9835,7 +9835,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -9875,7 +9875,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -9915,7 +9915,7 @@
         <v>29</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -9949,13 +9949,13 @@
         <v>30</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -9995,7 +9995,7 @@
         <v>35</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -10035,7 +10035,7 @@
         <v>165</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -10075,7 +10075,7 @@
         <v>129</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -10115,7 +10115,7 @@
         <v>146</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
@@ -10155,7 +10155,7 @@
         <v>147</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
@@ -10195,7 +10195,7 @@
         <v>145</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -10235,7 +10235,7 @@
         <v>144</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -10275,7 +10275,7 @@
         <v>143</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -10315,7 +10315,7 @@
         <v>141</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -10355,7 +10355,7 @@
         <v>142</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -10395,7 +10395,7 @@
         <v>149</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -10426,16 +10426,16 @@
     </row>
     <row r="31" spans="1:28">
       <c r="A31" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>218</v>
-      </c>
       <c r="C31" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -10445,7 +10445,7 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
@@ -10466,16 +10466,16 @@
     </row>
     <row r="32" spans="1:28">
       <c r="A32" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -10485,7 +10485,7 @@
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
@@ -10506,16 +10506,16 @@
     </row>
     <row r="33" spans="1:28">
       <c r="A33" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>241</v>
-      </c>
       <c r="C33" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
@@ -10525,7 +10525,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
       <c r="L33" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
@@ -10546,8 +10546,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ResponseDataType.gc" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -10562,8 +10562,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="12.75"/>
@@ -10577,7 +10577,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -10586,7 +10586,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -10595,7 +10595,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -10604,7 +10604,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="C4" s="14"/>
     </row>
@@ -10613,7 +10613,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -10622,7 +10622,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -10714,16 +10714,16 @@
     </row>
     <row r="8" spans="1:28">
       <c r="A8" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>224</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -10733,7 +10733,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
@@ -10754,16 +10754,16 @@
     </row>
     <row r="9" spans="1:28">
       <c r="A9" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>227</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -10773,7 +10773,7 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -10794,16 +10794,16 @@
     </row>
     <row r="10" spans="1:28">
       <c r="A10" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>230</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -10813,7 +10813,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
@@ -10834,16 +10834,16 @@
     </row>
     <row r="11" spans="1:28">
       <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>233</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -10853,7 +10853,7 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -10874,16 +10874,16 @@
     </row>
     <row r="12" spans="1:28">
       <c r="A12" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>236</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -10893,7 +10893,7 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -10914,16 +10914,16 @@
     </row>
     <row r="13" spans="1:28">
       <c r="A13" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>239</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -10933,7 +10933,7 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -10954,9 +10954,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId1" display="https://github.com/ESPD/ESPD-EDM" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId3" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/BooleanGUIControlType.gc" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -10985,7 +10985,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -10994,7 +10994,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -11003,7 +11003,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -11012,7 +11012,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -11021,7 +11021,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -11030,7 +11030,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -11039,7 +11039,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -11048,7 +11048,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -11057,7 +11057,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -11093,7 +11093,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -11103,7 +11103,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -11113,7 +11113,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11123,7 +11123,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11133,7 +11133,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11143,7 +11143,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="21"/>
@@ -11153,7 +11153,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11163,7 +11163,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -11173,7 +11173,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -11222,7 +11222,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -11232,7 +11232,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11242,7 +11242,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -11252,7 +11252,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11262,7 +11262,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11364,7 +11364,7 @@
         <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L8" t="s">
         <v>169</v>
@@ -11381,7 +11381,7 @@
         <v>170</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -11421,7 +11421,7 @@
         <v>171</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -11461,7 +11461,7 @@
         <v>172</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -11501,7 +11501,7 @@
         <v>173</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -11541,7 +11541,7 @@
         <v>174</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -11581,7 +11581,7 @@
         <v>175</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -11621,7 +11621,7 @@
         <v>176</v>
       </c>
       <c r="D15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L15" t="s">
         <v>176</v>
@@ -11638,7 +11638,7 @@
         <v>177</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -11678,7 +11678,7 @@
         <v>154</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -11718,7 +11718,7 @@
         <v>157</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -11749,8 +11749,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/CriterionElementType.gc" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -11779,7 +11779,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -11789,7 +11789,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -11799,7 +11799,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11809,7 +11809,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11819,7 +11819,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -11829,7 +11829,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11839,7 +11839,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11849,7 +11849,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -11859,7 +11859,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -11908,7 +11908,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -11918,7 +11918,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -11928,7 +11928,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11938,7 +11938,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11948,7 +11948,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11958,7 +11958,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11968,7 +11968,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11976,7 +11976,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -12012,7 +12012,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -12022,7 +12022,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -12032,7 +12032,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -12042,7 +12042,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -12052,7 +12052,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -12062,7 +12062,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12072,7 +12072,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12082,7 +12082,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -12092,7 +12092,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -12138,7 +12138,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -12148,7 +12148,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12158,7 +12158,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -12168,7 +12168,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -12178,7 +12178,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12280,7 +12280,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -12320,7 +12320,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -12360,7 +12360,7 @@
         <v>40</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -12400,7 +12400,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -12440,7 +12440,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="11"/>
@@ -12471,8 +12471,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/EOIDType.gc" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -12483,12 +12483,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12664,15 +12661,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12696,17 +12704,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>